<commit_message>
Added some more cases to the drawing algorithm
</commit_message>
<xml_diff>
--- a/Arthas.xlsx
+++ b/Arthas.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Arthas-II-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C58606-1B78-4201-B78E-86E9B98A676E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2477046-B095-4044-AE48-A3E090F0A985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EC5555B-C9D9-4C55-BE09-E1EC625CFAA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2EC5555B-C9D9-4C55-BE09-E1EC625CFAA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Track 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Track 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>Trecho</t>
   </si>
@@ -54,6 +54,27 @@
   <si>
     <t>Meia circunferência</t>
   </si>
+  <si>
+    <t>Turning direction</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Um quarto de circunferência</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right wheel</t>
+  </si>
+  <si>
+    <t>Left wheel</t>
+  </si>
+  <si>
+    <t>Distância entre eixos</t>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +109,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -112,11 +145,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +231,69 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -200,23 +365,71 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>417870</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>113694</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2051" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71769DE6-AACF-A564-AED1-5D45C898B6CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10972800" y="3429000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>93957</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>161213</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA6D22B-46A3-C3A5-FB99-F3BEAB2BA290}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E2B16B-07D7-7D44-EB1F-49357377EA62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -232,8 +445,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4600575" y="28575"/>
-          <a:ext cx="9838095" cy="4847619"/>
+          <a:off x="10477500" y="5705475"/>
+          <a:ext cx="10342857" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>960714</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E8F748-B6F4-6090-4BB9-863212B54888}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5715000"/>
+          <a:ext cx="10485714" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>884521</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>75502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6F5F89-2C69-E27F-C909-5BAC70F94BFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="5810250"/>
+          <a:ext cx="10428571" cy="5580952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -544,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75A450E-A5D3-412C-A345-B2F4D33A6851}">
   <dimension ref="C4:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,15 +1059,833 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDC10DD-18B8-4EC7-AFE4-17F7528F8C57}">
-  <dimension ref="A1"/>
+  <dimension ref="A5:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>130</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21">
+        <v>500</v>
+      </c>
+      <c r="F6" s="21">
+        <v>500</v>
+      </c>
+      <c r="G6" s="4">
+        <f>(140*E6)/(32*PI())</f>
+        <v>696.30287602704209</v>
+      </c>
+      <c r="H6" s="4">
+        <f>(140*F6)/(32*PI())</f>
+        <v>696.30287602704209</v>
+      </c>
+      <c r="K6" s="22">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="6">
+        <v>200</v>
+      </c>
+      <c r="N6" s="6">
+        <f>M6/2</f>
+        <v>100</v>
+      </c>
+      <c r="O6" s="6">
+        <f>2*PI()*N6</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P6" s="6">
+        <f>O6/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q6" s="7">
+        <f>P6/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21">
+        <v>250</v>
+      </c>
+      <c r="F7" s="21">
+        <v>250</v>
+      </c>
+      <c r="G7" s="4">
+        <f>(140*E7)/(32*PI())</f>
+        <v>348.15143801352104</v>
+      </c>
+      <c r="H7" s="4">
+        <f>(140*F7)/(32*PI())</f>
+        <v>348.15143801352104</v>
+      </c>
+      <c r="K7" s="22"/>
+      <c r="L7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="6">
+        <f>M6+A6</f>
+        <v>330</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" ref="N7:N8" si="0">M7/2</f>
+        <v>165</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" ref="O7:O8" si="1">2*PI()*N7</f>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P7" s="6">
+        <f t="shared" ref="P7:Q7" si="2">O7/2</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="2"/>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="21">
+        <f>Q7</f>
+        <v>259.18139392115791</v>
+      </c>
+      <c r="F8" s="21">
+        <f>Q8</f>
+        <v>54.977871437821378</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G13" si="3">(140*E8)/(32*PI())</f>
+        <v>360.9375</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ref="H8:H13" si="4">(140*F8)/(32*PI())</f>
+        <v>76.5625</v>
+      </c>
+      <c r="K8" s="23"/>
+      <c r="L8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="10">
+        <f>M6-A6</f>
+        <v>70</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="O8" s="10">
+        <f t="shared" si="1"/>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" ref="P8:Q8" si="5">O8/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q8" s="12">
+        <f t="shared" si="5"/>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="21">
+        <f>Q10</f>
+        <v>54.977871437821378</v>
+      </c>
+      <c r="F9" s="21">
+        <f>Q11</f>
+        <v>259.18139392115791</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="3"/>
+        <v>76.5625</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="4"/>
+        <v>360.9375</v>
+      </c>
+      <c r="K9" s="24">
+        <v>3</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="9">
+        <v>200</v>
+      </c>
+      <c r="N9" s="9">
+        <f>M9/2</f>
+        <v>100</v>
+      </c>
+      <c r="O9" s="9">
+        <f>2*PI()*N9</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P9" s="9">
+        <f>O9/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q9" s="13">
+        <f>P9/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="21">
+        <f>P13</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="F10" s="21">
+        <f>P14</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="3"/>
+        <v>721.875</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="4"/>
+        <v>153.125</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="6">
+        <f>M9-A6</f>
+        <v>70</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" ref="N10:N11" si="6">M10/2</f>
+        <v>35</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" ref="O10:O11" si="7">2*PI()*N10</f>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P10" s="6">
+        <f t="shared" ref="P10:Q10" si="8">O10/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="8"/>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="21">
+        <v>50</v>
+      </c>
+      <c r="F11" s="21">
+        <v>50</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="3"/>
+        <v>69.630287602704215</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="4"/>
+        <v>69.630287602704215</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="10">
+        <f>M9+A6</f>
+        <v>330</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="6"/>
+        <v>165</v>
+      </c>
+      <c r="O11" s="10">
+        <f t="shared" si="7"/>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" ref="P11:Q11" si="9">O11/2</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q11" s="16">
+        <f t="shared" si="9"/>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+      <c r="E12" s="21">
+        <f>Q16</f>
+        <v>54.977871437821378</v>
+      </c>
+      <c r="F12" s="21">
+        <f>Q17</f>
+        <v>259.18139392115791</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="3"/>
+        <v>76.5625</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="4"/>
+        <v>360.9375</v>
+      </c>
+      <c r="K12" s="25">
+        <v>4</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="9">
+        <v>200</v>
+      </c>
+      <c r="N12" s="9">
+        <f>M12/2</f>
+        <v>100</v>
+      </c>
+      <c r="O12" s="9">
+        <f>2*PI()*N12</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P12" s="14">
+        <f>O12/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q12" s="15">
+        <f>P12/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="21">
+        <v>50</v>
+      </c>
+      <c r="F13" s="21">
+        <v>50</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="3"/>
+        <v>69.630287602704215</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="4"/>
+        <v>69.630287602704215</v>
+      </c>
+      <c r="K13" s="22"/>
+      <c r="L13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="6">
+        <f>M12+A6</f>
+        <v>330</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" ref="N13:N14" si="10">M13/2</f>
+        <v>165</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" ref="O13:O14" si="11">2*PI()*N13</f>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" ref="P13:Q13" si="12">O13/2</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q13" s="8">
+        <f t="shared" si="12"/>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="8">
+        <f>P19</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="F14" s="3">
+        <f>P20</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" ref="G14" si="13">(140*E14)/(32*PI())</f>
+        <v>721.875</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" ref="H14" si="14">(140*F14)/(32*PI())</f>
+        <v>153.125</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="10">
+        <f>M12-A6</f>
+        <v>70</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="O14" s="10">
+        <f t="shared" si="11"/>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P14" s="16">
+        <f t="shared" ref="P14:Q14" si="15">O14/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="15"/>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3">
+        <v>250</v>
+      </c>
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" ref="G15" si="16">(140*E15)/(32*PI())</f>
+        <v>348.15143801352104</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" ref="H15" si="17">(140*F15)/(32*PI())</f>
+        <v>348.15143801352104</v>
+      </c>
+      <c r="K15" s="25">
+        <v>6</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="9">
+        <v>200</v>
+      </c>
+      <c r="N15" s="9">
+        <f>M15/2</f>
+        <v>100</v>
+      </c>
+      <c r="O15" s="9">
+        <f>2*PI()*N15</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P15" s="15">
+        <f>O15/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q15" s="14">
+        <f>P15/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <f>P22</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="F16" s="3">
+        <f>P23</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" ref="G16" si="18">(140*E16)/(32*PI())</f>
+        <v>153.125</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" ref="H16" si="19">(140*F16)/(32*PI())</f>
+        <v>721.875</v>
+      </c>
+      <c r="K16" s="22"/>
+      <c r="L16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="6">
+        <f>M15-$A$6</f>
+        <v>70</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" ref="N16:N17" si="20">M16/2</f>
+        <v>35</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" ref="O16:O17" si="21">2*PI()*N16</f>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P16" s="15">
+        <f t="shared" ref="P16:Q16" si="22">O16/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q16" s="14">
+        <f t="shared" si="22"/>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="10">
+        <f>M15+$A$6</f>
+        <v>330</v>
+      </c>
+      <c r="N17" s="18">
+        <f t="shared" si="20"/>
+        <v>165</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="21"/>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P17" s="19">
+        <f t="shared" ref="P17:Q17" si="23">O17/2</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q17" s="20">
+        <f t="shared" si="23"/>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="K18" s="25">
+        <v>8</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="9">
+        <v>200</v>
+      </c>
+      <c r="N18" s="9">
+        <f>M18/2</f>
+        <v>100</v>
+      </c>
+      <c r="O18" s="9">
+        <f>2*PI()*N18</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P18" s="14">
+        <f>O18/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>P18/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="6">
+        <f>M18+A6</f>
+        <v>330</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" ref="N19:N20" si="24">M19/2</f>
+        <v>165</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" ref="O19:O20" si="25">2*PI()*N19</f>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P19" s="7">
+        <f>O19/2</f>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q19" s="8">
+        <f t="shared" ref="P19:Q19" si="26">P19/2</f>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="3">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="10">
+        <f>M18-A6</f>
+        <v>70</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" si="24"/>
+        <v>35</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="25"/>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P20" s="16">
+        <f t="shared" ref="P20:Q20" si="27">O20/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q20" s="17">
+        <f t="shared" si="27"/>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="3">
+        <v>15</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="K21" s="25">
+        <v>6</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="9">
+        <v>200</v>
+      </c>
+      <c r="N21" s="9">
+        <f>M21/2</f>
+        <v>100</v>
+      </c>
+      <c r="O21" s="9">
+        <f>2*PI()*N21</f>
+        <v>628.31853071795865</v>
+      </c>
+      <c r="P21" s="14">
+        <f>O21/2</f>
+        <v>314.15926535897933</v>
+      </c>
+      <c r="Q21" s="15">
+        <f>P21/2</f>
+        <v>157.07963267948966</v>
+      </c>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D22" s="3">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="6">
+        <f>M21-$A$6</f>
+        <v>70</v>
+      </c>
+      <c r="N22" s="9">
+        <f t="shared" ref="N22:N23" si="28">M22/2</f>
+        <v>35</v>
+      </c>
+      <c r="O22" s="9">
+        <f t="shared" ref="O22:O23" si="29">2*PI()*N22</f>
+        <v>219.91148575128551</v>
+      </c>
+      <c r="P22" s="14">
+        <f t="shared" ref="P22:P23" si="30">O22/2</f>
+        <v>109.95574287564276</v>
+      </c>
+      <c r="Q22" s="15">
+        <f t="shared" ref="Q22:Q23" si="31">P22/2</f>
+        <v>54.977871437821378</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="3">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="10">
+        <f>M21+$A$6</f>
+        <v>330</v>
+      </c>
+      <c r="N23" s="18">
+        <f t="shared" si="28"/>
+        <v>165</v>
+      </c>
+      <c r="O23" s="18">
+        <f t="shared" si="29"/>
+        <v>1036.7255756846316</v>
+      </c>
+      <c r="P23" s="20">
+        <f t="shared" si="30"/>
+        <v>518.36278784231581</v>
+      </c>
+      <c r="Q23" s="19">
+        <f t="shared" si="31"/>
+        <v>259.18139392115791</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="3">
+        <v>18</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <v>19</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>20</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="K18:K20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="O6:O8 O12:O14 O9:O11 O15:O20" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>